<commit_message>
Етап 6 - excel
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2course\ООП\Інструменти і технології програмування\Лабораторна 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A6CC3F7-407D-4322-816A-3B5402303417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91720F9-A022-44F3-9FC5-022E5CA710F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{55D9D2AF-D7C0-4996-90AB-C5163840FA8A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="135  p p p" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,12 +31,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Бельгія</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Тест1</t>
+  </si>
+  <si>
+    <t>пор</t>
+  </si>
+  <si>
+    <t>Україна</t>
+  </si>
+  <si>
+    <t>Осв пр 1</t>
+  </si>
+  <si>
+    <t>kz</t>
+  </si>
+  <si>
+    <t>rti</t>
+  </si>
+  <si>
+    <t>dddd</t>
   </si>
 </sst>
 </file>
@@ -389,22 +404,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DCA901-C771-4F97-9BBC-C9D7EA13AF81}">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A2:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>